<commit_message>
First meeting update. Adjusted flowchart, created initial sketches, and created initial draft of Gannt chart.
</commit_message>
<xml_diff>
--- a/ganntChart.xlsx
+++ b/ganntChart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jared\OneDrive - Brigham Young University\BYU\6 - Fall 24\Process Control\balanceProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://byu-my.sharepoint.com/personal/jwp91_byu_edu/Documents/BYU/6 - Fall 24/Process Control/balanceProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D354F4F-64DE-4CD0-A148-589CB66A5E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="271" documentId="13_ncr:1_{3D354F4F-64DE-4CD0-A148-589CB66A5E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5630577F-7130-427F-B44A-B2241E72D8B9}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,19 +27,15 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={124DA08B-E699-4BF0-9622-21EFCBD5B151}</author>
+    <author>tc={BAC78219-F288-4D4C-B317-B87FC799D059}</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{124DA08B-E699-4BF0-9622-21EFCBD5B151}">
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{BAC78219-F288-4D4C-B317-B87FC799D059}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    - 2 servo motors
-- 1 ultrasonic sensor (already have 1, need 2)
-- 1 H-bridge (?)
-- 2 9V batteries &amp; hookups
-- ...others?</t>
+    Does I/O still work well with all components operating?</t>
       </text>
     </comment>
   </commentList>
@@ -47,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
   <si>
     <t>Item</t>
   </si>
@@ -79,23 +75,145 @@
     <t>Proposal</t>
   </si>
   <si>
-    <t>Buy parts</t>
-  </si>
-  <si>
-    <t>CAD: gearing system</t>
-  </si>
-  <si>
-    <t>Sketch system model</t>
-  </si>
-  <si>
-    <t>3D print gears</t>
+    <t>CAD: find Linear Actuator model</t>
+  </si>
+  <si>
+    <t>CAD: adjust model for our system</t>
+  </si>
+  <si>
+    <t>Print gears</t>
+  </si>
+  <si>
+    <t>Bootup Arduino</t>
+  </si>
+  <si>
+    <t>Install Thonny</t>
+  </si>
+  <si>
+    <t>Configure Minipython</t>
+  </si>
+  <si>
+    <t>Buy EcEn shop parts</t>
+  </si>
+  <si>
+    <t>Configure motors (on/off)</t>
+  </si>
+  <si>
+    <t>Test gearing w/motors</t>
+  </si>
+  <si>
+    <t>Configure motors (PWM)</t>
+  </si>
+  <si>
+    <t>Simultaneous motor test</t>
+  </si>
+  <si>
+    <t>Configure single US sensor</t>
+  </si>
+  <si>
+    <t>Configure dual US sensors</t>
+  </si>
+  <si>
+    <t>Determine y_min detector</t>
+  </si>
+  <si>
+    <t>Test limit signal</t>
+  </si>
+  <si>
+    <t>Confirm I/O</t>
+  </si>
+  <si>
+    <t>Size system based on:
+- Actuator limits
+- US sensor limits
+- Trough+ball mass</t>
+  </si>
+  <si>
+    <t>Test US sensor reading</t>
+  </si>
+  <si>
+    <t>Implement US filters</t>
+  </si>
+  <si>
+    <t>Create "getDavg" function</t>
+  </si>
+  <si>
+    <t>Test vertical limit enforcer reading</t>
+  </si>
+  <si>
+    <t>Create "check limit" function</t>
+  </si>
+  <si>
+    <t>Test motor actuation from code</t>
+  </si>
+  <si>
+    <t>Create "move" function</t>
+  </si>
+  <si>
+    <t>Assemble system</t>
+  </si>
+  <si>
+    <t>Create UI:
+- Auto/manual modes
+- Manual mode motor buttons</t>
+  </si>
+  <si>
+    <t>Test system with manual operation</t>
+  </si>
+  <si>
+    <t>Create main PID loop in code</t>
+  </si>
+  <si>
+    <t>Determine model for control loop</t>
+  </si>
+  <si>
+    <t>Test y_min enforcement</t>
+  </si>
+  <si>
+    <t>Test y_max behavior</t>
+  </si>
+  <si>
+    <t>Test US sensor readings</t>
+  </si>
+  <si>
+    <t>Determine PID parameters</t>
+  </si>
+  <si>
+    <t>Fune tuning</t>
+  </si>
+  <si>
+    <t>DOE to determine tuning params</t>
+  </si>
+  <si>
+    <t>Simultaneous component test</t>
+  </si>
+  <si>
+    <t>Source trough and ball</t>
+  </si>
+  <si>
+    <t>Week 1</t>
+  </si>
+  <si>
+    <t>Week 2</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>Week 4</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Week 6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,8 +227,17 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,8 +250,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -132,14 +289,129 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,180 +698,542 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B5" dT="2024-11-01T16:22:17.37" personId="{C586F1D8-EA9A-478D-945C-E3173CC6A56B}" id="{124DA08B-E699-4BF0-9622-21EFCBD5B151}">
-    <text>- 2 servo motors
-- 1 ultrasonic sensor (already have 1, need 2)
-- 1 H-bridge (?)
-- 2 9V batteries &amp; hookups
-- ...others?</text>
+  <threadedComment ref="B18" dT="2024-11-01T19:20:07.91" personId="{C586F1D8-EA9A-478D-945C-E3173CC6A56B}" id="{BAC78219-F288-4D4C-B317-B87FC799D059}">
+    <text>Does I/O still work well with all components operating?</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U27"/>
+  <dimension ref="A1:V47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.19921875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.19921875" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.19921875" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.19921875" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.19921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.19921875" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.19921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.19921875" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.19921875" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.19921875" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.19921875" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.19921875" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.9296875" style="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.9296875" style="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.9296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.9296875" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.9296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="38.73046875" style="3" customWidth="1"/>
+    <col min="22" max="22" width="6.59765625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:21" s="16" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="14"/>
+      <c r="D1" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="19"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="19"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="19"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="19"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="19"/>
+      <c r="U1" s="3"/>
+    </row>
+    <row r="2" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="5">
         <v>45597</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D2" s="21">
         <v>45600</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E2" s="22">
         <v>45602</v>
       </c>
-      <c r="F1" s="1">
+      <c r="F2" s="23">
         <v>45604</v>
       </c>
-      <c r="G1" s="1">
+      <c r="G2" s="6">
         <v>45607</v>
       </c>
-      <c r="H1" s="1">
+      <c r="H2" s="4">
         <v>45609</v>
       </c>
-      <c r="I1" s="1">
-        <v>45610</v>
-      </c>
-      <c r="J1" s="1">
+      <c r="I2" s="5">
         <v>45611</v>
       </c>
-      <c r="K1" s="1">
+      <c r="J2" s="4">
         <v>45614</v>
       </c>
-      <c r="L1" s="1">
+      <c r="K2" s="11">
         <v>45616</v>
       </c>
-      <c r="M1" s="1">
+      <c r="L2" s="5">
         <v>45618</v>
       </c>
-      <c r="N1" s="1">
+      <c r="M2" s="6">
         <v>45621</v>
       </c>
-      <c r="O1" s="1">
+      <c r="N2" s="11">
         <v>45623</v>
       </c>
-      <c r="P1" s="1">
+      <c r="O2" s="5">
         <v>45625</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="P2" s="6">
         <v>45628</v>
       </c>
-      <c r="R1" s="1">
+      <c r="Q2" s="11">
         <v>45630</v>
       </c>
-      <c r="S1" s="1">
+      <c r="R2" s="5">
         <v>45632</v>
       </c>
-      <c r="T1" s="1">
+      <c r="S2" s="21">
         <v>45635</v>
       </c>
-      <c r="U1" s="1">
+      <c r="T2" s="22">
         <v>45637</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="B2" t="s">
+      <c r="U2" s="3"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A3" s="25"/>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A4" s="25"/>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A5" s="25"/>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A6" s="25"/>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A7" s="25"/>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A8" s="25"/>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A9" s="25"/>
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A10" s="25"/>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A11" s="25"/>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A12" s="25"/>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A13" s="25"/>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+      <c r="A14" s="25"/>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A15" s="25"/>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A16" s="25"/>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A17" s="25"/>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A18" s="25"/>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A19" s="25"/>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="J19" s="1"/>
+      <c r="K19" s="13"/>
+    </row>
+    <row r="20" spans="1:15" ht="57" x14ac:dyDescent="0.45">
+      <c r="A20" s="25"/>
+      <c r="B20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" s="1"/>
+      <c r="K20" s="13"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A21" s="26"/>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="J21" s="1"/>
+      <c r="K21" s="13"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A22" s="26"/>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="J22" s="1"/>
+      <c r="K22" s="13"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A23" s="26"/>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="J23" s="1"/>
+      <c r="K23" s="13"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A24" s="26"/>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="J24" s="1"/>
+      <c r="K24" s="13"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A25" s="26"/>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="J25" s="1"/>
+      <c r="K25" s="13"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A26" s="26"/>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="J26" s="1"/>
+      <c r="K26" s="13"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A27" s="26"/>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="J27" s="1"/>
+      <c r="K27" s="13"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A28" s="26"/>
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+      <c r="J28" s="1"/>
+      <c r="K28" s="13"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A29" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B29" t="s">
         <v>9</v>
       </c>
-      <c r="M14" s="2"/>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+      <c r="L29" s="7"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A30" s="27"/>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="L30" s="7"/>
+      <c r="M30" s="8"/>
+    </row>
+    <row r="31" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A31" s="27"/>
+      <c r="B31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L31" s="7"/>
+      <c r="M31" s="8"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A32" s="27"/>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="N32" s="13"/>
+      <c r="O32" s="7"/>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A33" s="27"/>
+      <c r="B33" t="s">
+        <v>39</v>
+      </c>
+      <c r="N33" s="13"/>
+      <c r="O33" s="7"/>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A34" s="27"/>
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+      <c r="N34" s="13"/>
+      <c r="O34" s="7"/>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A35" s="27"/>
+      <c r="B35" t="s">
+        <v>41</v>
+      </c>
+      <c r="N35" s="13"/>
+      <c r="O35" s="7"/>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A36" s="27"/>
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+      <c r="N36" s="13"/>
+      <c r="O36" s="7"/>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A37" s="27"/>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="13"/>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A38" s="27"/>
+      <c r="B38" t="s">
+        <v>44</v>
+      </c>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="13"/>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A39" s="27"/>
+      <c r="B39" t="s">
+        <v>42</v>
+      </c>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="13"/>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A40" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B40" t="s">
         <v>7</v>
       </c>
-      <c r="R17" s="2"/>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+      <c r="Q40" s="13"/>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A41" s="27"/>
+      <c r="B41" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="7"/>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A42" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B42" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A43" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B43" t="s">
         <v>5</v>
       </c>
-      <c r="T23" s="2"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="T24" s="2"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+      <c r="S43" s="8"/>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A44" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B44" t="s">
         <v>1</v>
       </c>
-      <c r="U25" s="2"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+      <c r="T44" s="1"/>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A45" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B45" t="s">
         <v>4</v>
       </c>
-      <c r="U26" s="2"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+      <c r="T45" s="1"/>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A46" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B46" t="s">
         <v>8</v>
       </c>
-      <c r="U27" s="2"/>
+      <c r="T46" s="1"/>
+    </row>
+    <row r="47" spans="1:22" s="3" customFormat="1" ht="331.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C47" s="24"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="24"/>
+      <c r="I47" s="24"/>
+      <c r="J47" s="24"/>
+      <c r="K47" s="24"/>
+      <c r="L47" s="24"/>
+      <c r="M47" s="24"/>
+      <c r="N47" s="24"/>
+      <c r="O47" s="24"/>
+      <c r="P47" s="24"/>
+      <c r="Q47" s="24"/>
+      <c r="R47" s="24"/>
+      <c r="S47" s="24"/>
+      <c r="T47" s="24"/>
+      <c r="V47" s="16"/>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:O1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added link to ESP32 troubleshooting page. Updated Gannt chart
</commit_message>
<xml_diff>
--- a/ganntChart.xlsx
+++ b/ganntChart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://byu-my.sharepoint.com/personal/jwp91_byu_edu/Documents/BYU/6 - Fall 24/Process Control/balanceProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jared\OneDrive - Brigham Young University\BYU\6 - Fall 24\Process Control\balanceProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="271" documentId="13_ncr:1_{3D354F4F-64DE-4CD0-A148-589CB66A5E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5630577F-7130-427F-B44A-B2241E72D8B9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F695D2-F9AF-47EE-8583-8F73E4DB4420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -213,19 +213,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -237,7 +231,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,6 +271,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -373,45 +373,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="16" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="16" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,46 +708,44 @@
   <dimension ref="A1:V47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P30" sqref="P30"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="5.19921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.19921875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.19921875" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.19921875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.19921875" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.19921875" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.19921875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.19921875" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.19921875" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.19921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.19921875" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.19921875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.19921875" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.19921875" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.19921875" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.19921875" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.19921875" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.9296875" style="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.9296875" style="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.9296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.9296875" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.19921875" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="7.19921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.19921875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.19921875" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.19921875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.19921875" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.9296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.9296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.9296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.9296875" style="9" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6.9296875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="38.73046875" style="3" customWidth="1"/>
-    <col min="22" max="22" width="6.59765625" style="16"/>
+    <col min="21" max="21" width="38.73046875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="16" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:21" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
+      <c r="C1" s="10"/>
       <c r="D1" s="18" t="s">
         <v>47</v>
       </c>
@@ -778,388 +775,391 @@
         <v>52</v>
       </c>
       <c r="T1" s="19"/>
-      <c r="U1" s="3"/>
-    </row>
-    <row r="2" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="5">
+    </row>
+    <row r="2" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="4">
         <v>45597</v>
       </c>
-      <c r="D2" s="21">
+      <c r="D2" s="12">
         <v>45600</v>
       </c>
-      <c r="E2" s="22">
+      <c r="E2" s="13">
         <v>45602</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="14">
         <v>45604</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>45607</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>45609</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="4">
         <v>45611</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="3">
         <v>45614</v>
       </c>
-      <c r="K2" s="11">
+      <c r="K2" s="3">
         <v>45616</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="4">
         <v>45618</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="5">
         <v>45621</v>
       </c>
-      <c r="N2" s="11">
+      <c r="N2" s="3">
         <v>45623</v>
       </c>
-      <c r="O2" s="5">
+      <c r="O2" s="4">
         <v>45625</v>
       </c>
-      <c r="P2" s="6">
+      <c r="P2" s="5">
         <v>45628</v>
       </c>
-      <c r="Q2" s="11">
+      <c r="Q2" s="3">
         <v>45630</v>
       </c>
-      <c r="R2" s="5">
+      <c r="R2" s="4">
         <v>45632</v>
       </c>
-      <c r="S2" s="21">
+      <c r="S2" s="12">
         <v>45635</v>
       </c>
-      <c r="T2" s="22">
+      <c r="T2" s="13">
         <v>45637</v>
       </c>
-      <c r="U2" s="3"/>
+      <c r="U2" s="2"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A3" s="25"/>
+      <c r="A3" s="15"/>
       <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A4" s="25"/>
+      <c r="A4" s="15"/>
       <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A5" s="25"/>
+      <c r="A5" s="15"/>
       <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A6" s="25"/>
+      <c r="A6" s="15"/>
       <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A7" s="25"/>
+      <c r="A7" s="15"/>
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A8" s="25"/>
+      <c r="A8" s="15"/>
       <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A9" s="25"/>
+      <c r="A9" s="15"/>
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A10" s="25"/>
+      <c r="A10" s="15"/>
       <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="8"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="22"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A11" s="25"/>
+      <c r="A11" s="15"/>
       <c r="B11" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="8"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="26"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A12" s="25"/>
+      <c r="A12" s="15"/>
       <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="25"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A13" s="25"/>
+      <c r="A13" s="15"/>
       <c r="B13" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="1"/>
+      <c r="E13" s="26"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="25"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A14" s="25"/>
+      <c r="A14" s="15"/>
       <c r="B14" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="1"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="25"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A15" s="25"/>
+      <c r="A15" s="15"/>
       <c r="B15" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="1"/>
+      <c r="H15" s="25"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A16" s="25"/>
+      <c r="A16" s="15"/>
       <c r="B16" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="1"/>
+      <c r="H16" s="25"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A17" s="25"/>
+      <c r="A17" s="15"/>
       <c r="B17" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="7"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="23"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A18" s="25"/>
+      <c r="A18" s="15"/>
       <c r="B18" t="s">
         <v>45</v>
       </c>
-      <c r="I18" s="7"/>
+      <c r="I18" s="23"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A19" s="25"/>
+      <c r="A19" s="15"/>
       <c r="B19" t="s">
         <v>46</v>
       </c>
-      <c r="J19" s="1"/>
-      <c r="K19" s="13"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
     </row>
     <row r="20" spans="1:15" ht="57" x14ac:dyDescent="0.45">
-      <c r="A20" s="25"/>
-      <c r="B20" s="2" t="s">
+      <c r="A20" s="15"/>
+      <c r="B20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="1"/>
-      <c r="K20" s="13"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A21" s="26"/>
+      <c r="A21" s="16"/>
       <c r="B21" t="s">
         <v>25</v>
       </c>
-      <c r="J21" s="1"/>
-      <c r="K21" s="13"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A22" s="26"/>
+      <c r="A22" s="16"/>
       <c r="B22" t="s">
         <v>27</v>
       </c>
-      <c r="J22" s="1"/>
-      <c r="K22" s="13"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A23" s="26"/>
+      <c r="A23" s="16"/>
       <c r="B23" t="s">
         <v>28</v>
       </c>
-      <c r="J23" s="1"/>
-      <c r="K23" s="13"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A24" s="26"/>
+      <c r="A24" s="16"/>
       <c r="B24" t="s">
         <v>29</v>
       </c>
-      <c r="J24" s="1"/>
-      <c r="K24" s="13"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A25" s="26"/>
+      <c r="A25" s="16"/>
       <c r="B25" t="s">
         <v>30</v>
       </c>
-      <c r="J25" s="1"/>
-      <c r="K25" s="13"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A26" s="26"/>
+      <c r="A26" s="16"/>
       <c r="B26" t="s">
         <v>31</v>
       </c>
-      <c r="J26" s="1"/>
-      <c r="K26" s="13"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A27" s="26"/>
+      <c r="A27" s="16"/>
       <c r="B27" t="s">
         <v>32</v>
       </c>
-      <c r="J27" s="1"/>
-      <c r="K27" s="13"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A28" s="26"/>
+      <c r="A28" s="16"/>
       <c r="B28" t="s">
         <v>33</v>
       </c>
-      <c r="J28" s="1"/>
-      <c r="K28" s="13"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="16" t="s">
         <v>3</v>
       </c>
       <c r="B29" t="s">
         <v>9</v>
       </c>
-      <c r="L29" s="7"/>
+      <c r="L29" s="23"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A30" s="27"/>
+      <c r="A30" s="17"/>
       <c r="B30" t="s">
         <v>34</v>
       </c>
-      <c r="L30" s="7"/>
-      <c r="M30" s="8"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="22"/>
     </row>
     <row r="31" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A31" s="27"/>
-      <c r="B31" s="2" t="s">
+      <c r="A31" s="17"/>
+      <c r="B31" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L31" s="7"/>
-      <c r="M31" s="8"/>
+      <c r="L31" s="23"/>
+      <c r="M31" s="22"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A32" s="27"/>
+      <c r="A32" s="17"/>
       <c r="B32" t="s">
         <v>36</v>
       </c>
-      <c r="N32" s="13"/>
-      <c r="O32" s="7"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="23"/>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A33" s="27"/>
+      <c r="A33" s="17"/>
       <c r="B33" t="s">
         <v>39</v>
       </c>
-      <c r="N33" s="13"/>
-      <c r="O33" s="7"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="23"/>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A34" s="27"/>
+      <c r="A34" s="17"/>
       <c r="B34" t="s">
         <v>40</v>
       </c>
-      <c r="N34" s="13"/>
-      <c r="O34" s="7"/>
+      <c r="N34" s="24"/>
+      <c r="O34" s="23"/>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A35" s="27"/>
+      <c r="A35" s="17"/>
       <c r="B35" t="s">
         <v>41</v>
       </c>
-      <c r="N35" s="13"/>
-      <c r="O35" s="7"/>
+      <c r="N35" s="24"/>
+      <c r="O35" s="23"/>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A36" s="27"/>
+      <c r="A36" s="17"/>
       <c r="B36" t="s">
         <v>37</v>
       </c>
-      <c r="N36" s="13"/>
-      <c r="O36" s="7"/>
+      <c r="N36" s="24"/>
+      <c r="O36" s="23"/>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A37" s="27"/>
+      <c r="A37" s="17"/>
       <c r="B37" t="s">
         <v>38</v>
       </c>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="13"/>
+      <c r="P37" s="22"/>
+      <c r="Q37" s="24"/>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A38" s="27"/>
+      <c r="A38" s="17"/>
       <c r="B38" t="s">
         <v>44</v>
       </c>
-      <c r="P38" s="8"/>
-      <c r="Q38" s="13"/>
+      <c r="P38" s="22"/>
+      <c r="Q38" s="24"/>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A39" s="27"/>
+      <c r="A39" s="17"/>
       <c r="B39" t="s">
         <v>42</v>
       </c>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="13"/>
+      <c r="P39" s="22"/>
+      <c r="Q39" s="24"/>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A40" s="27" t="s">
+      <c r="A40" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
       </c>
-      <c r="Q40" s="13"/>
+      <c r="Q40" s="24"/>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A41" s="27"/>
+      <c r="A41" s="17"/>
       <c r="B41" t="s">
         <v>43</v>
       </c>
-      <c r="Q41" s="13"/>
-      <c r="R41" s="7"/>
+      <c r="Q41" s="24"/>
+      <c r="R41" s="23"/>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A42" s="27" t="s">
+      <c r="A42" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B42" t="s">
@@ -1167,61 +1167,43 @@
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A43" s="27" t="s">
+      <c r="A43" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B43" t="s">
         <v>5</v>
       </c>
-      <c r="S43" s="8"/>
+      <c r="S43" s="22"/>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B44" t="s">
         <v>1</v>
       </c>
-      <c r="T44" s="1"/>
+      <c r="T44" s="24"/>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A45" s="27" t="s">
+      <c r="A45" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B45" t="s">
         <v>4</v>
       </c>
-      <c r="T45" s="1"/>
+      <c r="T45" s="24"/>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A46" s="27" t="s">
+      <c r="A46" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B46" t="s">
         <v>8</v>
       </c>
-      <c r="T46" s="1"/>
-    </row>
-    <row r="47" spans="1:22" s="3" customFormat="1" ht="331.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="24"/>
-      <c r="H47" s="24"/>
-      <c r="I47" s="24"/>
-      <c r="J47" s="24"/>
-      <c r="K47" s="24"/>
-      <c r="L47" s="24"/>
-      <c r="M47" s="24"/>
-      <c r="N47" s="24"/>
-      <c r="O47" s="24"/>
-      <c r="P47" s="24"/>
-      <c r="Q47" s="24"/>
-      <c r="R47" s="24"/>
-      <c r="S47" s="24"/>
-      <c r="T47" s="24"/>
-      <c r="V47" s="16"/>
+      <c r="T46" s="24"/>
+    </row>
+    <row r="47" spans="1:22" s="2" customFormat="1" ht="331.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V47"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Tested 180deg servo and steppers. Successfully got both to spin, but realized quickly that fast 360 degree rotation is necessary, and neither of these can provide both.
</commit_message>
<xml_diff>
--- a/ganntChart.xlsx
+++ b/ganntChart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jared\OneDrive - Brigham Young University\BYU\6 - Fall 24\Process Control\balanceProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://byu-my.sharepoint.com/personal/jwp91_byu_edu/Documents/BYU/6 - Fall 24/Process Control/balanceProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F695D2-F9AF-47EE-8583-8F73E4DB4420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{B3F695D2-F9AF-47EE-8583-8F73E4DB4420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83DC650D-ED55-425E-9EF6-11E5D0D2576E}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -373,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -394,6 +394,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -406,11 +409,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -711,7 +710,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -739,46 +738,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="10"/>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="18" t="s">
+      <c r="E1" s="22"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="19"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="18" t="s">
+      <c r="H1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="19"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="18" t="s">
+      <c r="K1" s="22"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="19"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="18" t="s">
+      <c r="N1" s="22"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="18" t="s">
+      <c r="Q1" s="22"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="T1" s="19"/>
+      <c r="T1" s="22"/>
     </row>
     <row r="2" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
       <c r="C2" s="4">
         <v>45597</v>
       </c>
@@ -864,38 +863,38 @@
       <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="22"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" s="15"/>
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="22"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A8" s="15"/>
       <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="22"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="7"/>
       <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A9" s="15"/>
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="22"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="F9" s="20"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A10" s="15"/>
@@ -903,154 +902,150 @@
         <v>18</v>
       </c>
       <c r="E10" s="25"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="22"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A11" s="15"/>
       <c r="B11" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="26"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A12" s="15"/>
       <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="26"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="25"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="20"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A13" s="15"/>
       <c r="B13" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="26"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="25"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="20"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A14" s="15"/>
       <c r="B14" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="22"/>
-      <c r="H14" s="25"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="20"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A15" s="15"/>
       <c r="B15" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="25"/>
+      <c r="H15" s="20"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A16" s="15"/>
       <c r="B16" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="25"/>
+      <c r="H16" s="20"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" s="15"/>
       <c r="B17" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="26"/>
-      <c r="I17" s="23"/>
+      <c r="I17" s="19"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18" s="15"/>
       <c r="B18" t="s">
         <v>45</v>
       </c>
-      <c r="I18" s="23"/>
+      <c r="I18" s="19"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19" s="15"/>
       <c r="B19" t="s">
         <v>46</v>
       </c>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
     </row>
     <row r="20" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A20" s="15"/>
       <c r="B20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A21" s="16"/>
       <c r="B21" t="s">
         <v>25</v>
       </c>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A22" s="16"/>
       <c r="B22" t="s">
         <v>27</v>
       </c>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A23" s="16"/>
       <c r="B23" t="s">
         <v>28</v>
       </c>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A24" s="16"/>
       <c r="B24" t="s">
         <v>29</v>
       </c>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A25" s="16"/>
       <c r="B25" t="s">
         <v>30</v>
       </c>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A26" s="16"/>
       <c r="B26" t="s">
         <v>31</v>
       </c>
-      <c r="J26" s="24"/>
-      <c r="K26" s="24"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A27" s="16"/>
       <c r="B27" t="s">
         <v>32</v>
       </c>
-      <c r="J27" s="24"/>
-      <c r="K27" s="24"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A28" s="16"/>
       <c r="B28" t="s">
         <v>33</v>
       </c>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A29" s="16" t="s">
@@ -1059,87 +1054,87 @@
       <c r="B29" t="s">
         <v>9</v>
       </c>
-      <c r="L29" s="23"/>
+      <c r="L29" s="19"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A30" s="17"/>
       <c r="B30" t="s">
         <v>34</v>
       </c>
-      <c r="L30" s="23"/>
-      <c r="M30" s="22"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="18"/>
     </row>
     <row r="31" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A31" s="17"/>
       <c r="B31" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L31" s="23"/>
-      <c r="M31" s="22"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="18"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A32" s="17"/>
       <c r="B32" t="s">
         <v>36</v>
       </c>
-      <c r="N32" s="24"/>
-      <c r="O32" s="23"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="19"/>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A33" s="17"/>
       <c r="B33" t="s">
         <v>39</v>
       </c>
-      <c r="N33" s="24"/>
-      <c r="O33" s="23"/>
+      <c r="N33" s="20"/>
+      <c r="O33" s="19"/>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A34" s="17"/>
       <c r="B34" t="s">
         <v>40</v>
       </c>
-      <c r="N34" s="24"/>
-      <c r="O34" s="23"/>
+      <c r="N34" s="20"/>
+      <c r="O34" s="19"/>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A35" s="17"/>
       <c r="B35" t="s">
         <v>41</v>
       </c>
-      <c r="N35" s="24"/>
-      <c r="O35" s="23"/>
+      <c r="N35" s="20"/>
+      <c r="O35" s="19"/>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A36" s="17"/>
       <c r="B36" t="s">
         <v>37</v>
       </c>
-      <c r="N36" s="24"/>
-      <c r="O36" s="23"/>
+      <c r="N36" s="20"/>
+      <c r="O36" s="19"/>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A37" s="17"/>
       <c r="B37" t="s">
         <v>38</v>
       </c>
-      <c r="P37" s="22"/>
-      <c r="Q37" s="24"/>
+      <c r="P37" s="18"/>
+      <c r="Q37" s="20"/>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A38" s="17"/>
       <c r="B38" t="s">
         <v>44</v>
       </c>
-      <c r="P38" s="22"/>
-      <c r="Q38" s="24"/>
+      <c r="P38" s="18"/>
+      <c r="Q38" s="20"/>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A39" s="17"/>
       <c r="B39" t="s">
         <v>42</v>
       </c>
-      <c r="P39" s="22"/>
-      <c r="Q39" s="24"/>
+      <c r="P39" s="18"/>
+      <c r="Q39" s="20"/>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A40" s="17" t="s">
@@ -1148,15 +1143,15 @@
       <c r="B40" t="s">
         <v>7</v>
       </c>
-      <c r="Q40" s="24"/>
+      <c r="Q40" s="20"/>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A41" s="17"/>
       <c r="B41" t="s">
         <v>43</v>
       </c>
-      <c r="Q41" s="24"/>
-      <c r="R41" s="23"/>
+      <c r="Q41" s="20"/>
+      <c r="R41" s="19"/>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A42" s="17" t="s">
@@ -1173,7 +1168,7 @@
       <c r="B43" t="s">
         <v>5</v>
       </c>
-      <c r="S43" s="22"/>
+      <c r="S43" s="18"/>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A44" s="17" t="s">
@@ -1182,7 +1177,7 @@
       <c r="B44" t="s">
         <v>1</v>
       </c>
-      <c r="T44" s="24"/>
+      <c r="T44" s="20"/>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A45" s="17" t="s">
@@ -1191,7 +1186,7 @@
       <c r="B45" t="s">
         <v>4</v>
       </c>
-      <c r="T45" s="24"/>
+      <c r="T45" s="20"/>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A46" s="17" t="s">
@@ -1200,7 +1195,7 @@
       <c r="B46" t="s">
         <v>8</v>
       </c>
-      <c r="T46" s="24"/>
+      <c r="T46" s="20"/>
     </row>
     <row r="47" spans="1:22" s="2" customFormat="1" ht="331.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="V47"/>

</xml_diff>

<commit_message>
Created a physics-based simulation of the system.
</commit_message>
<xml_diff>
--- a/ganntChart.xlsx
+++ b/ganntChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://byu-my.sharepoint.com/personal/jwp91_byu_edu/Documents/BYU/6 - Fall 24/Process Control/balanceProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{B3F695D2-F9AF-47EE-8583-8F73E4DB4420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C29DB87-017E-4230-AFF3-C1869612C81F}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{B3F695D2-F9AF-47EE-8583-8F73E4DB4420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D7BC8CE-CA7F-44D6-9638-1655914C0C1C}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <author>tc={BAC78219-F288-4D4C-B317-B87FC799D059}</author>
   </authors>
   <commentList>
-    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{BAC78219-F288-4D4C-B317-B87FC799D059}">
+    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{BAC78219-F288-4D4C-B317-B87FC799D059}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>Item</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>Configure motors (PWM)</t>
-  </si>
-  <si>
-    <t>Simultaneous motor test</t>
   </si>
   <si>
     <t>Configure single US sensor</t>
@@ -696,7 +693,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B18" dT="2024-11-01T19:20:07.91" personId="{C586F1D8-EA9A-478D-945C-E3173CC6A56B}" id="{BAC78219-F288-4D4C-B317-B87FC799D059}">
+  <threadedComment ref="B17" dT="2024-11-01T19:20:07.91" personId="{C586F1D8-EA9A-478D-945C-E3173CC6A56B}" id="{BAC78219-F288-4D4C-B317-B87FC799D059}">
     <text>Does I/O still work well with all components operating?</text>
   </threadedComment>
 </ThreadedComments>
@@ -704,13 +701,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V47"/>
+  <dimension ref="A1:V46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -746,32 +743,32 @@
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E1" s="23"/>
       <c r="F1" s="24"/>
       <c r="G1" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H1" s="23"/>
       <c r="I1" s="24"/>
       <c r="J1" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K1" s="23"/>
       <c r="L1" s="24"/>
       <c r="M1" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N1" s="23"/>
       <c r="O1" s="24"/>
       <c r="P1" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q1" s="23"/>
       <c r="R1" s="24"/>
       <c r="S1" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="T1" s="23"/>
     </row>
@@ -926,7 +923,7 @@
     <row r="13" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A13" s="15"/>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G13" s="18"/>
       <c r="H13" s="20"/>
@@ -934,10 +931,9 @@
     <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A14" s="15"/>
       <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="18"/>
-      <c r="H14" s="20"/>
+        <v>20</v>
+      </c>
+      <c r="H14" s="21"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A15" s="15"/>
@@ -949,14 +945,14 @@
     <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A16" s="15"/>
       <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="20"/>
+        <v>23</v>
+      </c>
+      <c r="I16" s="19"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" s="15"/>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="I17" s="19"/>
     </row>
@@ -965,20 +961,21 @@
       <c r="B18" t="s">
         <v>45</v>
       </c>
-      <c r="I18" s="19"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+    </row>
+    <row r="19" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A19" s="15"/>
-      <c r="B19" t="s">
-        <v>46</v>
-      </c>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-    </row>
-    <row r="20" spans="1:15" ht="57" x14ac:dyDescent="0.45">
-      <c r="A20" s="15"/>
-      <c r="B20" s="1" t="s">
-        <v>26</v>
+      <c r="B19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A20" s="16"/>
+      <c r="B20" t="s">
+        <v>24</v>
       </c>
       <c r="J20" s="20"/>
       <c r="K20" s="20"/>
@@ -986,7 +983,7 @@
     <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A21" s="16"/>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
@@ -1040,42 +1037,42 @@
       <c r="K27" s="20"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A28" s="16"/>
+      <c r="A28" s="16" t="s">
+        <v>3</v>
+      </c>
       <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="L28" s="19"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A29" s="17"/>
+      <c r="B29" t="s">
         <v>33</v>
       </c>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A29" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" t="s">
-        <v>9</v>
-      </c>
       <c r="L29" s="19"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M29" s="18"/>
+    </row>
+    <row r="30" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A30" s="17"/>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>34</v>
       </c>
       <c r="L30" s="19"/>
       <c r="M30" s="18"/>
     </row>
-    <row r="31" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A31" s="17"/>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>35</v>
       </c>
-      <c r="L31" s="19"/>
-      <c r="M31" s="18"/>
+      <c r="N31" s="20"/>
+      <c r="O31" s="19"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A32" s="17"/>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N32" s="20"/>
       <c r="O32" s="19"/>
@@ -1099,7 +1096,7 @@
     <row r="35" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A35" s="17"/>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="N35" s="20"/>
       <c r="O35" s="19"/>
@@ -1109,13 +1106,13 @@
       <c r="B36" t="s">
         <v>37</v>
       </c>
-      <c r="N36" s="20"/>
-      <c r="O36" s="19"/>
+      <c r="P36" s="18"/>
+      <c r="Q36" s="20"/>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A37" s="17"/>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="P37" s="18"/>
       <c r="Q37" s="20"/>
@@ -1123,59 +1120,60 @@
     <row r="38" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A38" s="17"/>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P38" s="18"/>
       <c r="Q38" s="20"/>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A39" s="17"/>
+      <c r="A39" s="17" t="s">
+        <v>3</v>
+      </c>
       <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q39" s="20"/>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A40" s="17"/>
+      <c r="B40" t="s">
         <v>42</v>
       </c>
-      <c r="P39" s="18"/>
-      <c r="Q39" s="20"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A40" s="17" t="s">
+      <c r="Q40" s="20"/>
+      <c r="R40" s="19"/>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A41" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B40" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q40" s="20"/>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A41" s="17"/>
       <c r="B41" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q41" s="20"/>
-      <c r="R41" s="19"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A42" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="S42" s="18"/>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A43" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
-      </c>
-      <c r="S43" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="T43" s="20"/>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A44" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="T44" s="20"/>
     </row>
@@ -1184,21 +1182,12 @@
         <v>3</v>
       </c>
       <c r="B45" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="T45" s="20"/>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A46" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B46" t="s">
-        <v>8</v>
-      </c>
-      <c r="T46" s="20"/>
-    </row>
-    <row r="47" spans="1:22" s="2" customFormat="1" ht="331.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V47"/>
+    <row r="46" spans="1:22" s="2" customFormat="1" ht="331.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V46"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>